<commit_message>
update docs Definition of Done y Sprint Backlog
</commit_message>
<xml_diff>
--- a/docs/Sprint Backlog.xlsx
+++ b/docs/Sprint Backlog.xlsx
@@ -5,18 +5,29 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdmor\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RESER-REEF\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3F6B81-0411-48B2-B6B8-BB3F66CF558C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{764F42F6-85BD-415F-9020-7A0E04CDE6D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog 01" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="PmA1bboWR0bJoIo3DKSnQ8hB3QynDf4hB405ZMG0mqE="/>
     </ext>
@@ -263,9 +274,6 @@
     <t>REGISTRO DE USUARIOS Y AUTENTICACIÓN</t>
   </si>
   <si>
-    <t>E3-HU9</t>
-  </si>
-  <si>
     <t>Creación de cuenta</t>
   </si>
   <si>
@@ -573,6 +581,9 @@
   </si>
   <si>
     <t>En curso</t>
+  </si>
+  <si>
+    <t>E2-HU9</t>
   </si>
 </sst>
 </file>
@@ -652,7 +663,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -687,6 +698,30 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -917,7 +952,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1082,12 +1117,43 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFF99"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1300,10 +1366,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB1022"/>
+  <dimension ref="A1:BT1022"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F2" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1323,7 +1389,7 @@
     <col min="13" max="28" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:72" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
@@ -1357,7 +1423,7 @@
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
     </row>
-    <row r="2" spans="1:28" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:72" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1411,7 +1477,7 @@
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
     </row>
-    <row r="3" spans="1:28" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:72" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>14</v>
       </c>
@@ -1445,7 +1511,7 @@
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
     </row>
-    <row r="4" spans="1:28" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:72" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>16</v>
       </c>
@@ -1480,7 +1546,7 @@
         <v>23</v>
       </c>
       <c r="L4" s="18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M4" s="13"/>
       <c r="N4" s="1"/>
@@ -1499,7 +1565,7 @@
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
     </row>
-    <row r="5" spans="1:28" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:72" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>25</v>
       </c>
@@ -1534,7 +1600,7 @@
         <v>23</v>
       </c>
       <c r="L5" s="21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M5" s="13"/>
       <c r="N5" s="1"/>
@@ -1553,7 +1619,7 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
     </row>
-    <row r="6" spans="1:28" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:72" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>31</v>
       </c>
@@ -1588,7 +1654,7 @@
         <v>23</v>
       </c>
       <c r="L6" s="21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M6" s="13"/>
       <c r="N6" s="1"/>
@@ -1607,7 +1673,7 @@
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
     </row>
-    <row r="7" spans="1:28" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:72" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>36</v>
       </c>
@@ -1641,7 +1707,7 @@
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
     </row>
-    <row r="8" spans="1:28" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:72" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>38</v>
       </c>
@@ -1676,7 +1742,7 @@
         <v>23</v>
       </c>
       <c r="L8" s="21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M8" s="13"/>
       <c r="N8" s="1"/>
@@ -1695,7 +1761,7 @@
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
     </row>
-    <row r="9" spans="1:28" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:72" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>43</v>
       </c>
@@ -1730,7 +1796,7 @@
         <v>23</v>
       </c>
       <c r="L9" s="21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M9" s="13"/>
       <c r="N9" s="1"/>
@@ -1749,7 +1815,7 @@
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
     </row>
-    <row r="10" spans="1:28" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:72" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>48</v>
       </c>
@@ -1783,7 +1849,7 @@
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
     </row>
-    <row r="11" spans="1:28" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:72" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>50</v>
       </c>
@@ -1818,7 +1884,7 @@
         <v>23</v>
       </c>
       <c r="L11" s="21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M11" s="13"/>
       <c r="N11" s="1"/>
@@ -1837,7 +1903,7 @@
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
     </row>
-    <row r="12" spans="1:28" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:72" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>55</v>
       </c>
@@ -1872,7 +1938,7 @@
         <v>23</v>
       </c>
       <c r="L12" s="21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M12" s="13"/>
       <c r="N12" s="1"/>
@@ -1891,7 +1957,7 @@
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
     </row>
-    <row r="13" spans="1:28" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:72" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
         <v>60</v>
       </c>
@@ -1926,7 +1992,7 @@
         <v>23</v>
       </c>
       <c r="L13" s="21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M13" s="13"/>
       <c r="N13" s="1"/>
@@ -1945,7 +2011,7 @@
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
     </row>
-    <row r="14" spans="1:28" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:72" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>65</v>
       </c>
@@ -1979,78 +2045,122 @@
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
     </row>
-    <row r="15" spans="1:28" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:72" s="61" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="B15" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="C15" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="D15" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="E15" s="64" t="s">
         <v>70</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="F15" s="65" t="s">
         <v>71</v>
       </c>
-      <c r="F15" s="25" t="s">
+      <c r="G15" s="66">
+        <v>5</v>
+      </c>
+      <c r="H15" s="66">
+        <v>2</v>
+      </c>
+      <c r="I15" s="66">
+        <v>1</v>
+      </c>
+      <c r="J15" s="66">
+        <v>2</v>
+      </c>
+      <c r="K15" s="66" t="s">
+        <v>23</v>
+      </c>
+      <c r="L15" s="60" t="s">
+        <v>169</v>
+      </c>
+      <c r="M15" s="67"/>
+      <c r="N15" s="68"/>
+      <c r="O15" s="68"/>
+      <c r="P15" s="68"/>
+      <c r="Q15" s="68"/>
+      <c r="R15" s="68"/>
+      <c r="S15" s="68"/>
+      <c r="T15" s="68"/>
+      <c r="U15" s="68"/>
+      <c r="V15" s="68"/>
+      <c r="W15" s="68"/>
+      <c r="X15" s="68"/>
+      <c r="Y15" s="68"/>
+      <c r="Z15" s="68"/>
+      <c r="AA15" s="68"/>
+      <c r="AB15" s="68"/>
+      <c r="AC15" s="69"/>
+      <c r="AD15" s="69"/>
+      <c r="AE15" s="69"/>
+      <c r="AF15" s="69"/>
+      <c r="AG15" s="69"/>
+      <c r="AH15" s="69"/>
+      <c r="AI15" s="69"/>
+      <c r="AJ15" s="69"/>
+      <c r="AK15" s="69"/>
+      <c r="AL15" s="69"/>
+      <c r="AM15" s="69"/>
+      <c r="AN15" s="69"/>
+      <c r="AO15" s="69"/>
+      <c r="AP15" s="69"/>
+      <c r="AQ15" s="69"/>
+      <c r="AR15" s="69"/>
+      <c r="AS15" s="69"/>
+      <c r="AT15" s="69"/>
+      <c r="AU15" s="69"/>
+      <c r="AV15" s="69"/>
+      <c r="AW15" s="69"/>
+      <c r="AX15" s="69"/>
+      <c r="AY15" s="69"/>
+      <c r="AZ15" s="69"/>
+      <c r="BA15" s="69"/>
+      <c r="BB15" s="69"/>
+      <c r="BC15" s="69"/>
+      <c r="BD15" s="69"/>
+      <c r="BE15" s="69"/>
+      <c r="BF15" s="69"/>
+      <c r="BG15" s="69"/>
+      <c r="BH15" s="69"/>
+      <c r="BI15" s="69"/>
+      <c r="BJ15" s="69"/>
+      <c r="BK15" s="69"/>
+      <c r="BL15" s="69"/>
+      <c r="BM15" s="69"/>
+      <c r="BN15" s="69"/>
+      <c r="BO15" s="69"/>
+      <c r="BP15" s="69"/>
+      <c r="BQ15" s="69"/>
+      <c r="BR15" s="69"/>
+      <c r="BS15" s="69"/>
+      <c r="BT15" s="69"/>
+    </row>
+    <row r="16" spans="1:72" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="G15" s="21">
-        <v>5</v>
-      </c>
-      <c r="H15" s="21">
-        <v>2</v>
-      </c>
-      <c r="I15" s="21">
-        <v>1</v>
-      </c>
-      <c r="J15" s="21">
-        <v>2</v>
-      </c>
-      <c r="K15" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="L15" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="M15" s="13"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
-      <c r="T15" s="1"/>
-      <c r="U15" s="1"/>
-      <c r="V15" s="1"/>
-      <c r="W15" s="1"/>
-      <c r="X15" s="1"/>
-      <c r="Y15" s="1"/>
-      <c r="Z15" s="1"/>
-      <c r="AA15" s="1"/>
-      <c r="AB15" s="1"/>
-    </row>
-    <row r="16" spans="1:28" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="14" t="s">
+      <c r="B16" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="C16" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="D16" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="E16" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="30" t="s">
         <v>76</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="F16" s="30" t="s">
-        <v>77</v>
       </c>
       <c r="G16" s="31">
         <v>3</v>
@@ -2068,7 +2178,7 @@
         <v>23</v>
       </c>
       <c r="L16" s="31" t="s">
-        <v>169</v>
+        <v>24</v>
       </c>
       <c r="M16" s="13"/>
       <c r="N16" s="1"/>
@@ -2089,10 +2199,10 @@
     </row>
     <row r="17" spans="1:28" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>78</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>79</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="10"/>
@@ -2123,22 +2233,22 @@
     </row>
     <row r="18" spans="1:28" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="B18" s="29" t="s">
+      <c r="C18" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="D18" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="E18" s="18" t="s">
+      <c r="F18" s="30" t="s">
         <v>83</v>
-      </c>
-      <c r="F18" s="30" t="s">
-        <v>84</v>
       </c>
       <c r="G18" s="34">
         <v>8</v>
@@ -2156,7 +2266,7 @@
         <v>23</v>
       </c>
       <c r="L18" s="31" t="s">
-        <v>169</v>
+        <v>24</v>
       </c>
       <c r="M18" s="13"/>
       <c r="N18" s="1"/>
@@ -2177,22 +2287,22 @@
     </row>
     <row r="19" spans="1:28" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="C19" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="D19" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="D19" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="E19" s="17" t="s">
+      <c r="F19" s="30" t="s">
         <v>88</v>
-      </c>
-      <c r="F19" s="30" t="s">
-        <v>89</v>
       </c>
       <c r="G19" s="34">
         <v>8</v>
@@ -2210,7 +2320,7 @@
         <v>23</v>
       </c>
       <c r="L19" s="31" t="s">
-        <v>169</v>
+        <v>24</v>
       </c>
       <c r="M19" s="13"/>
       <c r="N19" s="1"/>
@@ -2231,22 +2341,22 @@
     </row>
     <row r="20" spans="1:28" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="C20" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="D20" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="F20" s="30" t="s">
         <v>92</v>
-      </c>
-      <c r="D20" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="F20" s="30" t="s">
-        <v>93</v>
       </c>
       <c r="G20" s="34">
         <v>13</v>
@@ -2264,7 +2374,7 @@
         <v>23</v>
       </c>
       <c r="L20" s="31" t="s">
-        <v>169</v>
+        <v>24</v>
       </c>
       <c r="M20" s="13"/>
       <c r="N20" s="1"/>
@@ -2285,22 +2395,22 @@
     </row>
     <row r="21" spans="1:28" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="B21" s="29" t="s">
+      <c r="C21" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="D21" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="D21" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="E21" s="18" t="s">
+      <c r="F21" s="30" t="s">
         <v>97</v>
-      </c>
-      <c r="F21" s="30" t="s">
-        <v>98</v>
       </c>
       <c r="G21" s="34">
         <v>13</v>
@@ -2318,7 +2428,7 @@
         <v>23</v>
       </c>
       <c r="L21" s="31" t="s">
-        <v>169</v>
+        <v>24</v>
       </c>
       <c r="M21" s="13"/>
       <c r="N21" s="1"/>
@@ -2339,10 +2449,10 @@
     </row>
     <row r="22" spans="1:28" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>99</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>100</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="10"/>
@@ -2373,22 +2483,22 @@
     </row>
     <row r="23" spans="1:28" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="C23" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="C23" s="29" t="s">
+      <c r="D23" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="D23" s="33" t="s">
+      <c r="E23" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="E23" s="18" t="s">
+      <c r="F23" s="30" t="s">
         <v>105</v>
-      </c>
-      <c r="F23" s="30" t="s">
-        <v>106</v>
       </c>
       <c r="G23" s="34">
         <v>8</v>
@@ -2403,10 +2513,10 @@
         <v>5</v>
       </c>
       <c r="K23" s="31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L23" s="31" t="s">
-        <v>169</v>
+        <v>24</v>
       </c>
       <c r="M23" s="13"/>
       <c r="N23" s="1"/>
@@ -2427,22 +2537,22 @@
     </row>
     <row r="24" spans="1:28" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B24" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="B24" s="29" t="s">
+      <c r="C24" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="D24" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="D24" s="33" t="s">
+      <c r="E24" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="E24" s="17" t="s">
+      <c r="F24" s="30" t="s">
         <v>112</v>
-      </c>
-      <c r="F24" s="30" t="s">
-        <v>113</v>
       </c>
       <c r="G24" s="34">
         <v>8</v>
@@ -2457,10 +2567,10 @@
         <v>5</v>
       </c>
       <c r="K24" s="31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L24" s="31" t="s">
-        <v>169</v>
+        <v>24</v>
       </c>
       <c r="M24" s="13"/>
       <c r="N24" s="1"/>
@@ -2481,22 +2591,22 @@
     </row>
     <row r="25" spans="1:28" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25" s="37" t="s">
         <v>114</v>
       </c>
-      <c r="B25" s="37" t="s">
+      <c r="C25" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="C25" s="29" t="s">
+      <c r="D25" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="D25" s="38" t="s">
+      <c r="E25" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="F25" s="30" t="s">
         <v>117</v>
-      </c>
-      <c r="E25" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="F25" s="30" t="s">
-        <v>118</v>
       </c>
       <c r="G25" s="34">
         <v>5</v>
@@ -2511,10 +2621,10 @@
         <v>45813</v>
       </c>
       <c r="K25" s="34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L25" s="31" t="s">
-        <v>170</v>
+        <v>24</v>
       </c>
       <c r="M25" s="13"/>
       <c r="N25" s="1"/>
@@ -2535,10 +2645,10 @@
     </row>
     <row r="26" spans="1:28" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>119</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>120</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="10"/>
@@ -2569,22 +2679,22 @@
     </row>
     <row r="27" spans="1:28" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B27" s="37" t="s">
         <v>121</v>
       </c>
-      <c r="B27" s="37" t="s">
+      <c r="C27" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="C27" s="29" t="s">
+      <c r="D27" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="D27" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="E27" s="39" t="s">
+      <c r="F27" s="30" t="s">
         <v>124</v>
-      </c>
-      <c r="F27" s="30" t="s">
-        <v>125</v>
       </c>
       <c r="G27" s="34">
         <v>8</v>
@@ -2602,7 +2712,7 @@
         <v>23</v>
       </c>
       <c r="L27" s="31" t="s">
-        <v>170</v>
+        <v>24</v>
       </c>
       <c r="M27" s="13"/>
       <c r="N27" s="1"/>
@@ -2623,22 +2733,22 @@
     </row>
     <row r="28" spans="1:28" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="B28" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="B28" s="37" t="s">
+      <c r="C28" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="C28" s="29" t="s">
+      <c r="D28" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E28" s="40" t="s">
         <v>128</v>
       </c>
-      <c r="D28" s="33" t="s">
-        <v>111</v>
-      </c>
-      <c r="E28" s="40" t="s">
+      <c r="F28" s="30" t="s">
         <v>129</v>
-      </c>
-      <c r="F28" s="30" t="s">
-        <v>130</v>
       </c>
       <c r="G28" s="34">
         <v>13</v>
@@ -2656,7 +2766,7 @@
         <v>23</v>
       </c>
       <c r="L28" s="31" t="s">
-        <v>170</v>
+        <v>24</v>
       </c>
       <c r="M28" s="13"/>
       <c r="N28" s="1"/>
@@ -2677,22 +2787,22 @@
     </row>
     <row r="29" spans="1:28" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B29" s="37" t="s">
         <v>131</v>
       </c>
-      <c r="B29" s="37" t="s">
+      <c r="C29" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="C29" s="29" t="s">
+      <c r="D29" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" s="41" t="s">
         <v>133</v>
       </c>
-      <c r="D29" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="E29" s="41" t="s">
+      <c r="F29" s="30" t="s">
         <v>134</v>
-      </c>
-      <c r="F29" s="30" t="s">
-        <v>135</v>
       </c>
       <c r="G29" s="31">
         <v>5</v>
@@ -2707,7 +2817,7 @@
         <v>45844</v>
       </c>
       <c r="K29" s="34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L29" s="31" t="s">
         <v>24</v>
@@ -2731,10 +2841,10 @@
     </row>
     <row r="30" spans="1:28" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B30" s="8" t="s">
         <v>136</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>137</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="22"/>
@@ -2765,22 +2875,22 @@
     </row>
     <row r="31" spans="1:28" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B31" s="42" t="s">
         <v>138</v>
       </c>
-      <c r="B31" s="42" t="s">
+      <c r="C31" s="43" t="s">
         <v>139</v>
       </c>
-      <c r="C31" s="43" t="s">
+      <c r="D31" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="D31" s="18" t="s">
+      <c r="E31" s="41" t="s">
         <v>141</v>
       </c>
-      <c r="E31" s="41" t="s">
+      <c r="F31" s="30" t="s">
         <v>142</v>
-      </c>
-      <c r="F31" s="30" t="s">
-        <v>143</v>
       </c>
       <c r="G31" s="34">
         <v>8</v>
@@ -2819,22 +2929,22 @@
     </row>
     <row r="32" spans="1:28" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="B32" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="B32" s="42" t="s">
+      <c r="C32" s="43" t="s">
         <v>145</v>
       </c>
-      <c r="C32" s="43" t="s">
+      <c r="D32" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="D32" s="18" t="s">
+      <c r="E32" s="41" t="s">
         <v>147</v>
       </c>
-      <c r="E32" s="41" t="s">
+      <c r="F32" s="30" t="s">
         <v>148</v>
-      </c>
-      <c r="F32" s="30" t="s">
-        <v>149</v>
       </c>
       <c r="G32" s="34">
         <v>8</v>
@@ -2849,7 +2959,7 @@
         <v>7</v>
       </c>
       <c r="K32" s="34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L32" s="31" t="s">
         <v>24</v>
@@ -2873,22 +2983,22 @@
     </row>
     <row r="33" spans="1:28" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B33" s="42" t="s">
         <v>151</v>
       </c>
-      <c r="B33" s="42" t="s">
+      <c r="C33" s="43" t="s">
         <v>152</v>
       </c>
-      <c r="C33" s="43" t="s">
+      <c r="D33" s="18" t="s">
         <v>153</v>
       </c>
-      <c r="D33" s="18" t="s">
+      <c r="E33" s="41" t="s">
         <v>154</v>
       </c>
-      <c r="E33" s="41" t="s">
+      <c r="F33" s="30" t="s">
         <v>155</v>
-      </c>
-      <c r="F33" s="30" t="s">
-        <v>156</v>
       </c>
       <c r="G33" s="34">
         <v>5</v>
@@ -2903,7 +3013,7 @@
         <v>7</v>
       </c>
       <c r="K33" s="34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L33" s="31" t="s">
         <v>24</v>
@@ -2927,22 +3037,22 @@
     </row>
     <row r="34" spans="1:28" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="B34" s="42" t="s">
         <v>157</v>
       </c>
-      <c r="B34" s="42" t="s">
+      <c r="C34" s="43" t="s">
         <v>158</v>
       </c>
-      <c r="C34" s="43" t="s">
+      <c r="D34" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="D34" s="18" t="s">
+      <c r="E34" s="41" t="s">
         <v>160</v>
       </c>
-      <c r="E34" s="41" t="s">
+      <c r="F34" s="30" t="s">
         <v>161</v>
-      </c>
-      <c r="F34" s="30" t="s">
-        <v>162</v>
       </c>
       <c r="G34" s="34">
         <v>5</v>
@@ -2981,22 +3091,22 @@
     </row>
     <row r="35" spans="1:28" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="B35" s="42" t="s">
         <v>163</v>
       </c>
-      <c r="B35" s="42" t="s">
+      <c r="C35" s="43" t="s">
         <v>164</v>
       </c>
-      <c r="C35" s="43" t="s">
+      <c r="D35" s="18" t="s">
         <v>165</v>
       </c>
-      <c r="D35" s="18" t="s">
+      <c r="E35" s="41" t="s">
         <v>166</v>
       </c>
-      <c r="E35" s="41" t="s">
+      <c r="F35" s="17" t="s">
         <v>167</v>
-      </c>
-      <c r="F35" s="17" t="s">
-        <v>168</v>
       </c>
       <c r="G35" s="31">
         <v>3</v>

</xml_diff>